<commit_message>
change format for file sensor
</commit_message>
<xml_diff>
--- a/Philip_Example_Of_Data.xlsx
+++ b/Philip_Example_Of_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hieph/Library/CloudStorage/Dropbox/HIEP/EDUCATION/HAMK/2024/DF_Project_HTML/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hieph/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FFF9C65-0C4C-5E42-A8A8-87069963A5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B102FB1-94A4-FE4A-881D-7AB297BFCD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{359AD550-4520-554E-B8E3-950CDC9EFC2E}"/>
   </bookViews>
@@ -540,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0E54D2-09AC-D349-A3F4-8E24C42F8F94}">
-  <dimension ref="A2:O22"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M22"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,59 +560,103 @@
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2">
+        <v>452.88799999999998</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="F2" s="2">
+        <v>60.816139999999997</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2">
+        <v>23.623370000000001</v>
+      </c>
+      <c r="J2" s="2">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>13</v>
+      <c r="K2" s="2">
+        <v>7.952998</v>
+      </c>
+      <c r="L2" s="2">
+        <v>16</v>
+      </c>
+      <c r="M2" s="2">
+        <v>21.8125</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>452.88799999999998</v>
+        <v>202.95529999999999</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -639,25 +683,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J3" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K3" s="2">
-        <v>7.952998</v>
+        <v>7.8606160000000003</v>
       </c>
       <c r="L3" s="2">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="M3" s="2">
-        <v>21.8125</v>
+        <v>21.9375</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>202.95529999999999</v>
+        <v>388.1859</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -684,25 +728,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J4" s="2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="K4" s="2">
-        <v>7.8606160000000003</v>
+        <v>7.831442</v>
       </c>
       <c r="L4" s="2">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M4" s="2">
-        <v>21.9375</v>
+        <v>22.125</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>388.1859</v>
+        <v>429.95650000000001</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -729,25 +773,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J5" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="K5" s="2">
         <v>7.831442</v>
       </c>
       <c r="L5" s="2">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="M5" s="2">
         <v>22.125</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>429.95650000000001</v>
+        <v>192.55260000000001</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
@@ -774,25 +818,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J6" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K6" s="2">
-        <v>7.831442</v>
+        <v>7.8168550000000003</v>
       </c>
       <c r="L6" s="2">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="M6" s="2">
-        <v>22.125</v>
+        <v>22.1875</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>192.55260000000001</v>
+        <v>191.31610000000001</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -819,25 +863,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J7" s="2">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K7" s="2">
         <v>7.8168550000000003</v>
       </c>
       <c r="L7" s="2">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="M7" s="2">
         <v>22.1875</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>191.31610000000001</v>
+        <v>186.9676</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
@@ -849,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2">
         <v>60.816139999999997</v>
@@ -864,25 +908,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J8" s="2">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K8" s="2">
         <v>7.8168550000000003</v>
       </c>
       <c r="L8" s="2">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="M8" s="2">
         <v>22.1875</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>186.9676</v>
+        <v>187.5908</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
@@ -909,25 +953,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J9" s="2">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="K9" s="2">
-        <v>7.8168550000000003</v>
+        <v>7.826568</v>
       </c>
       <c r="L9" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M9" s="2">
         <v>22.1875</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>187.5908</v>
+        <v>186.34370000000001</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
@@ -954,25 +998,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J10" s="2">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K10" s="2">
-        <v>7.826568</v>
+        <v>7.8217179999999997</v>
       </c>
       <c r="L10" s="2">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="M10" s="2">
-        <v>22.1875</v>
+        <v>22.25</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>186.34370000000001</v>
+        <v>185.09389999999999</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
@@ -999,25 +1043,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J11" s="2">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K11" s="2">
         <v>7.8217179999999997</v>
       </c>
       <c r="L11" s="2">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="M11" s="2">
         <v>22.25</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>185.09389999999999</v>
+        <v>183.21430000000001</v>
       </c>
       <c r="B12" s="2">
         <v>2</v>
@@ -1044,19 +1088,19 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J12" s="2">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="K12" s="2">
         <v>7.8217179999999997</v>
       </c>
       <c r="L12" s="2">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="M12" s="2">
         <v>22.25</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O12" s="2"/>
     </row>
@@ -1089,19 +1133,19 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J13" s="2">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K13" s="2">
         <v>7.8217179999999997</v>
       </c>
       <c r="L13" s="2">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="M13" s="2">
         <v>22.25</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O13" s="2"/>
     </row>
@@ -1134,25 +1178,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J14" s="2">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="K14" s="2">
         <v>7.8217179999999997</v>
       </c>
       <c r="L14" s="2">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="M14" s="2">
         <v>22.25</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>183.21430000000001</v>
+        <v>182.5865</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -1179,25 +1223,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J15" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K15" s="2">
-        <v>7.8217179999999997</v>
+        <v>7.8168550000000003</v>
       </c>
       <c r="L15" s="2">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M15" s="2">
-        <v>22.25</v>
+        <v>22.1875</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>182.5865</v>
+        <v>181.9579</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
@@ -1224,25 +1268,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J16" s="2">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K16" s="2">
         <v>7.8168550000000003</v>
       </c>
       <c r="L16" s="2">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="M16" s="2">
         <v>22.1875</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>181.9579</v>
+        <v>181.3288</v>
       </c>
       <c r="B17" s="2">
         <v>2</v>
@@ -1269,25 +1313,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J17" s="2">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="K17" s="2">
         <v>7.8168550000000003</v>
       </c>
       <c r="L17" s="2">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="M17" s="2">
         <v>22.1875</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>181.3288</v>
+        <v>180.69890000000001</v>
       </c>
       <c r="B18" s="2">
         <v>2</v>
@@ -1314,25 +1358,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J18" s="2">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="K18" s="2">
         <v>7.8168550000000003</v>
       </c>
       <c r="L18" s="2">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M18" s="2">
         <v>22.1875</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>180.69890000000001</v>
+        <v>180.0684</v>
       </c>
       <c r="B19" s="2">
         <v>2</v>
@@ -1344,7 +1388,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2">
         <v>60.816139999999997</v>
@@ -1359,25 +1403,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J19" s="2">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="K19" s="2">
-        <v>7.8168550000000003</v>
+        <v>7.7585750000000004</v>
       </c>
       <c r="L19" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="M19" s="2">
-        <v>22.1875</v>
+        <v>22.125</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>180.0684</v>
+        <v>181.3288</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
@@ -1404,25 +1448,25 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J20" s="2">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="K20" s="2">
-        <v>7.7585750000000004</v>
+        <v>7.8168550000000003</v>
       </c>
       <c r="L20" s="2">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="M20" s="2">
         <v>22.125</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>181.3288</v>
+        <v>180.69890000000001</v>
       </c>
       <c r="B21" s="2">
         <v>2</v>
@@ -1449,66 +1493,21 @@
         <v>23.623370000000001</v>
       </c>
       <c r="J21" s="2">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="K21" s="2">
-        <v>7.8168550000000003</v>
+        <v>7.8068780000000002</v>
       </c>
       <c r="L21" s="2">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="M21" s="2">
         <v>22.125</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>180.69890000000001</v>
-      </c>
-      <c r="B22" s="2">
-        <v>2</v>
-      </c>
-      <c r="C22" s="2">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2">
-        <v>2</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2</v>
-      </c>
-      <c r="F22" s="2">
-        <v>60.816139999999997</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="2">
-        <v>23.623370000000001</v>
-      </c>
-      <c r="J22" s="2">
-        <v>30</v>
-      </c>
-      <c r="K22" s="2">
-        <v>7.8068780000000002</v>
-      </c>
-      <c r="L22" s="2">
-        <v>20</v>
-      </c>
-      <c r="M22" s="2">
-        <v>22.125</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>